<commit_message>
Commited on 200524 23:13
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/testdata.xlsx
+++ b/src/test/resources/excel/testdata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ragus\IdeaProjects\E-CommerceOpenSource\src\test\resources\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD00CDF6-BD25-4BD6-9541-CF539BFD11E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A5427D5-D02D-46A7-92B0-483AB0E35005}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1848" yWindow="1848" windowWidth="17280" windowHeight="8880" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Runner" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="25">
   <si>
     <t>Test name</t>
   </si>
@@ -88,10 +88,19 @@
     <t>aded</t>
   </si>
   <si>
-    <t>No</t>
-  </si>
-  <si>
-    <t>NO</t>
+    <t>To verify login functionality with invalid credentials</t>
+  </si>
+  <si>
+    <t>Browser</t>
+  </si>
+  <si>
+    <t>firefox</t>
+  </si>
+  <si>
+    <t>edge</t>
+  </si>
+  <si>
+    <t>chrome</t>
   </si>
 </sst>
 </file>
@@ -152,10 +161,10 @@
   </cellStyleXfs>
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -436,33 +445,33 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="52.21875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="7.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
     </row>
@@ -476,10 +485,10 @@
       <c r="C2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="1" t="s">
         <v>9</v>
       </c>
     </row>
@@ -493,10 +502,27 @@
       <c r="C3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="E3" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" s="1" t="s">
         <v>9</v>
       </c>
     </row>
@@ -507,10 +533,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A1B6BC2-B1CD-4F2F-BBBE-801FCCC50BF4}">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -520,60 +546,72 @@
     <col min="3" max="3" width="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="2" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" s="3" t="s">
+      <c r="E1" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D2" s="3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="13.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="3" t="s">
+      <c r="D2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="13.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D3" s="3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" s="3" t="s">
+      <c r="D3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D4" s="1" t="s">
         <v>7</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
bestSellers,newRelease and moverAndShakers Tests and related pages are created and unwanted pages are removed on 25-05-24
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/testdata.xlsx
+++ b/src/test/resources/excel/testdata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ragus\IdeaProjects\E-CommerceOpenSource\src\test\resources\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A5427D5-D02D-46A7-92B0-483AB0E35005}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8A9F820-6835-4A43-AA84-452874FBB9DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1848" yWindow="1848" windowWidth="17280" windowHeight="8880" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="35">
   <si>
     <t>Test name</t>
   </si>
@@ -91,9 +91,6 @@
     <t>To verify login functionality with invalid credentials</t>
   </si>
   <si>
-    <t>Browser</t>
-  </si>
-  <si>
     <t>firefox</t>
   </si>
   <si>
@@ -101,6 +98,39 @@
   </si>
   <si>
     <t>chrome</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>To verity header of the page is correct or not</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>menutext</t>
+  </si>
+  <si>
+    <t>browser</t>
+  </si>
+  <si>
+    <t>New Releases</t>
+  </si>
+  <si>
+    <t>newReleaseTest</t>
+  </si>
+  <si>
+    <t>bestSellersTest</t>
+  </si>
+  <si>
+    <t>Movers and Shakers</t>
+  </si>
+  <si>
+    <t>Best Sellers</t>
+  </si>
+  <si>
+    <t>moversandShakersTest</t>
   </si>
 </sst>
 </file>
@@ -159,12 +189,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -445,15 +473,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="A5" sqref="A5:F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.77734375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="52.21875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="7.5546875" bestFit="1" customWidth="1"/>
   </cols>
@@ -483,7 +511,7 @@
         <v>6</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>7</v>
+        <v>24</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>9</v>
@@ -500,7 +528,7 @@
         <v>8</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>7</v>
+        <v>24</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>10</v>
@@ -517,12 +545,63 @@
         <v>20</v>
       </c>
       <c r="C4" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E4" s="1" t="s">
+      <c r="D5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E7" s="1" t="s">
         <v>9</v>
       </c>
     </row>
@@ -533,20 +612,21 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A1B6BC2-B1CD-4F2F-BBBE-801FCCC50BF4}">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9" customWidth="1"/>
+    <col min="6" max="6" width="17.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>15</v>
       </c>
@@ -559,11 +639,14 @@
       <c r="D1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="E1" s="3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E1" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
@@ -574,13 +657,16 @@
         <v>17</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E2" s="4" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" ht="13.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E2" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="13.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>11</v>
       </c>
@@ -591,13 +677,16 @@
         <v>17</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+        <v>24</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>18</v>
       </c>
@@ -608,10 +697,73 @@
         <v>19</v>
       </c>
       <c r="D4" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D5" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E4" s="4" t="s">
-        <v>23</v>
+      <c r="E5" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
set descriptions for each tests which will be appeared in extent report
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/testdata.xlsx
+++ b/src/test/resources/excel/testdata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ragus\IdeaProjects\E-CommerceOpenSource\src\test\resources\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8A9F820-6835-4A43-AA84-452874FBB9DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8641F1C-DB5F-47EE-A1AE-C339CC9A9301}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1848" yWindow="1848" windowWidth="17280" windowHeight="8880" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Runner" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="33">
   <si>
     <t>Test name</t>
   </si>
@@ -46,21 +46,12 @@
     <t>loginTest</t>
   </si>
   <si>
-    <t>To verify login functionality with valid credentials</t>
-  </si>
-  <si>
     <t>Yes</t>
   </si>
   <si>
-    <t xml:space="preserve">To verify login functionality with valid credentials via logi Test </t>
-  </si>
-  <si>
     <t>1</t>
   </si>
   <si>
-    <t>2</t>
-  </si>
-  <si>
     <t>logoutTest</t>
   </si>
   <si>
@@ -88,9 +79,6 @@
     <t>aded</t>
   </si>
   <si>
-    <t>To verify login functionality with invalid credentials</t>
-  </si>
-  <si>
     <t>firefox</t>
   </si>
   <si>
@@ -103,9 +91,6 @@
     <t>No</t>
   </si>
   <si>
-    <t>To verity header of the page is correct or not</t>
-  </si>
-  <si>
     <t/>
   </si>
   <si>
@@ -131,6 +116,15 @@
   </si>
   <si>
     <t>moversandShakersTest</t>
+  </si>
+  <si>
+    <t>To verity header of the best sellers page is correct or not</t>
+  </si>
+  <si>
+    <t>To verity header of the new release page is correct or not</t>
+  </si>
+  <si>
+    <t>To verity header of the mover and shaker page is correct or not</t>
   </si>
 </sst>
 </file>
@@ -473,16 +467,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:F7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="22.77734375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="52.21875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="53.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="7.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -505,104 +499,53 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>5</v>
+        <v>26</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>6</v>
+        <v>30</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>11</v>
+        <v>25</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>8</v>
+        <v>31</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>24</v>
+        <v>6</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>18</v>
+        <v>29</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>20</v>
+        <v>32</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>24</v>
+        <v>6</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C5" s="1" t="s">
         <v>7</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A6" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A7" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>9</v>
       </c>
     </row>
   </sheetData>
@@ -614,7 +557,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A1B6BC2-B1CD-4F2F-BBBE-801FCCC50BF4}">
   <dimension ref="A1:F7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
@@ -628,22 +571,22 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
@@ -651,119 +594,119 @@
         <v>5</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="13.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D3" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>21</v>
-      </c>
       <c r="F3" s="1" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E4" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>22</v>
-      </c>
       <c r="F4" s="1" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
docker-compose.yaml file is created for dockerized selenium grid
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/testdata.xlsx
+++ b/src/test/resources/excel/testdata.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27628"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ragus\IdeaProjects\E-CommerceOpenSource\src\test\resources\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8641F1C-DB5F-47EE-A1AE-C339CC9A9301}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EFC3336-D673-46F2-9837-E6C89F3F0728}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="27">
   <si>
     <t>Test name</t>
   </si>
@@ -43,21 +43,12 @@
     <t>Count</t>
   </si>
   <si>
-    <t>loginTest</t>
-  </si>
-  <si>
     <t>Yes</t>
   </si>
   <si>
     <t>1</t>
   </si>
   <si>
-    <t>logoutTest</t>
-  </si>
-  <si>
-    <t>Admin</t>
-  </si>
-  <si>
     <t>password</t>
   </si>
   <si>
@@ -70,15 +61,6 @@
     <t>username</t>
   </si>
   <si>
-    <t>admin123</t>
-  </si>
-  <si>
-    <t>loginTestInValid</t>
-  </si>
-  <si>
-    <t>aded</t>
-  </si>
-  <si>
     <t>firefox</t>
   </si>
   <si>
@@ -88,9 +70,6 @@
     <t>chrome</t>
   </si>
   <si>
-    <t>No</t>
-  </si>
-  <si>
     <t/>
   </si>
   <si>
@@ -125,6 +104,9 @@
   </si>
   <si>
     <t>To verity header of the mover and shaker page is correct or not</t>
+  </si>
+  <si>
+    <t>yes</t>
   </si>
 </sst>
 </file>
@@ -183,10 +165,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -470,7 +453,7 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -499,53 +482,53 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="C3" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="1" t="s">
-        <v>7</v>
-      </c>
       <c r="E3" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="C4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="1" t="s">
-        <v>7</v>
-      </c>
       <c r="E4" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>
@@ -555,10 +538,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A1B6BC2-B1CD-4F2F-BBBE-801FCCC50BF4}">
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -571,142 +554,82 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E3" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D1" s="2" t="s">
+      <c r="F3" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E4" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="E1" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D2" s="1" t="s">
+      <c r="F4" s="3" t="s">
         <v>20</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="13.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A5" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A6" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A7" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Dockerized selenium grid setup
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/testdata.xlsx
+++ b/src/test/resources/excel/testdata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ragus\IdeaProjects\E-CommerceOpenSource\src\test\resources\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EFC3336-D673-46F2-9837-E6C89F3F0728}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E098B8DA-79AC-47E0-91E9-6C512573905B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1848" yWindow="1848" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Runner" sheetId="1" r:id="rId1"/>
@@ -70,40 +70,40 @@
     <t>chrome</t>
   </si>
   <si>
+    <t>menutext</t>
+  </si>
+  <si>
+    <t>browser</t>
+  </si>
+  <si>
+    <t>New Releases</t>
+  </si>
+  <si>
+    <t>newReleaseTest</t>
+  </si>
+  <si>
+    <t>bestSellersTest</t>
+  </si>
+  <si>
+    <t>Movers and Shakers</t>
+  </si>
+  <si>
+    <t>Best Sellers</t>
+  </si>
+  <si>
+    <t>moversandShakersTest</t>
+  </si>
+  <si>
+    <t>To verity header of the best sellers page is correct or not</t>
+  </si>
+  <si>
+    <t>To verity header of the new release page is correct or not</t>
+  </si>
+  <si>
+    <t>To verity header of the mover and shaker page is correct or not</t>
+  </si>
+  <si>
     <t/>
-  </si>
-  <si>
-    <t>menutext</t>
-  </si>
-  <si>
-    <t>browser</t>
-  </si>
-  <si>
-    <t>New Releases</t>
-  </si>
-  <si>
-    <t>newReleaseTest</t>
-  </si>
-  <si>
-    <t>bestSellersTest</t>
-  </si>
-  <si>
-    <t>Movers and Shakers</t>
-  </si>
-  <si>
-    <t>Best Sellers</t>
-  </si>
-  <si>
-    <t>moversandShakersTest</t>
-  </si>
-  <si>
-    <t>To verity header of the best sellers page is correct or not</t>
-  </si>
-  <si>
-    <t>To verity header of the new release page is correct or not</t>
-  </si>
-  <si>
-    <t>To verity header of the mover and shaker page is correct or not</t>
   </si>
   <si>
     <t>yes</t>
@@ -165,11 +165,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -453,7 +452,7 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -482,10 +481,10 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>5</v>
@@ -499,13 +498,13 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>26</v>
+        <v>5</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>6</v>
@@ -516,10 +515,10 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>5</v>
@@ -541,7 +540,7 @@
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+      <selection activeCell="A2" sqref="A2:F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -566,70 +565,70 @@
         <v>8</v>
       </c>
       <c r="E1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F3" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="F1" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A2" s="3" t="s">
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F4" s="1" t="s">
         <v>19</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A3" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A4" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>